<commit_message>
Added random drop support.
</commit_message>
<xml_diff>
--- a/Documentation/Items and Enemies.xlsx
+++ b/Documentation/Items and Enemies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jopatterson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTDLS\RougueQuest\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B29664B-2B9B-4872-9BA1-88358B4778A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF1C82-E60A-4E08-BECA-C93A7FB71A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="265">
   <si>
     <t>Name</t>
   </si>
@@ -198,126 +198,129 @@
     <t>2 Slot Belt</t>
   </si>
   <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>3 Slot Belt</t>
+  </si>
+  <si>
+    <t>4 Slot Belt</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>5 Slot Belt</t>
+  </si>
+  <si>
+    <t>Ultra Rare</t>
+  </si>
+  <si>
+    <t>Mana</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Cast Fireball</t>
+  </si>
+  <si>
+    <t>Permanently learn Cast Fireball</t>
+  </si>
+  <si>
+    <t>Cast Poison</t>
+  </si>
+  <si>
+    <t>Permanently learn Cast Poison</t>
+  </si>
+  <si>
+    <t>Constitution</t>
+  </si>
+  <si>
+    <t>Permanently learn Constitution</t>
+  </si>
+  <si>
+    <t>Cure Poison</t>
+  </si>
+  <si>
+    <t>Permanently learn Cure Poison</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Permanently learn Defense</t>
+  </si>
+  <si>
+    <t>Permanently learn Dexterity</t>
+  </si>
+  <si>
+    <t>Earth Resistance</t>
+  </si>
+  <si>
+    <t>Permanently learn Earth Resistance</t>
+  </si>
+  <si>
+    <t>Electric Resistance</t>
+  </si>
+  <si>
+    <t>Permanently learn Electric Resistance</t>
+  </si>
+  <si>
+    <t>Fire Resistance</t>
+  </si>
+  <si>
+    <t>Permanently learn Fire Resistance</t>
+  </si>
+  <si>
+    <t>Heal Major Woulds</t>
+  </si>
+  <si>
+    <t>Permanently learn Heal Major Woulds</t>
+  </si>
+  <si>
+    <t>Heal Medium Woulds</t>
+  </si>
+  <si>
+    <t>Permanently learn Heal Medium Woulds</t>
+  </si>
+  <si>
+    <t>Heal Minor Woulds</t>
+  </si>
+  <si>
+    <t>Permanently learn Heal Minor Woulds</t>
+  </si>
+  <si>
+    <t>Hold Monster</t>
+  </si>
+  <si>
+    <t>Permanently learn Hold Monster</t>
+  </si>
+  <si>
+    <t>Ice Resistance</t>
+  </si>
+  <si>
+    <t>Permanently learn Ice Resistance</t>
+  </si>
+  <si>
+    <t>Magic Arrow</t>
+  </si>
+  <si>
+    <t>Permanently learn Magic Arrow</t>
+  </si>
+  <si>
+    <t>Permanently learn Strength</t>
+  </si>
+  <si>
+    <t>NameLevel</t>
+  </si>
+  <si>
+    <t>Leather Boots</t>
+  </si>
+  <si>
     <t>Common</t>
   </si>
   <si>
-    <t>3 Slot Belt</t>
-  </si>
-  <si>
-    <t>4 Slot Belt</t>
-  </si>
-  <si>
-    <t>5 Slot Belt</t>
-  </si>
-  <si>
-    <t>Uncommon</t>
-  </si>
-  <si>
-    <t>Mana</t>
-  </si>
-  <si>
-    <t>Effect</t>
-  </si>
-  <si>
-    <t>Cast Fireball</t>
-  </si>
-  <si>
-    <t>Ultra Rare</t>
-  </si>
-  <si>
-    <t>Permanently learn Cast Fireball</t>
-  </si>
-  <si>
-    <t>Cast Poison</t>
-  </si>
-  <si>
-    <t>Permanently learn Cast Poison</t>
-  </si>
-  <si>
-    <t>Constitution</t>
-  </si>
-  <si>
-    <t>Permanently learn Constitution</t>
-  </si>
-  <si>
-    <t>Cure Poison</t>
-  </si>
-  <si>
-    <t>Permanently learn Cure Poison</t>
-  </si>
-  <si>
-    <t>Defense</t>
-  </si>
-  <si>
-    <t>Permanently learn Defense</t>
-  </si>
-  <si>
-    <t>Permanently learn Dexterity</t>
-  </si>
-  <si>
-    <t>Earth Resistance</t>
-  </si>
-  <si>
-    <t>Permanently learn Earth Resistance</t>
-  </si>
-  <si>
-    <t>Electric Resistance</t>
-  </si>
-  <si>
-    <t>Permanently learn Electric Resistance</t>
-  </si>
-  <si>
-    <t>Fire Resistance</t>
-  </si>
-  <si>
-    <t>Permanently learn Fire Resistance</t>
-  </si>
-  <si>
-    <t>Heal Major Woulds</t>
-  </si>
-  <si>
-    <t>Permanently learn Heal Major Woulds</t>
-  </si>
-  <si>
-    <t>Heal Medium Woulds</t>
-  </si>
-  <si>
-    <t>Permanently learn Heal Medium Woulds</t>
-  </si>
-  <si>
-    <t>Heal Minor Woulds</t>
-  </si>
-  <si>
-    <t>Permanently learn Heal Minor Woulds</t>
-  </si>
-  <si>
-    <t>Hold Monster</t>
-  </si>
-  <si>
-    <t>Permanently learn Hold Monster</t>
-  </si>
-  <si>
-    <t>Ice Resistance</t>
-  </si>
-  <si>
-    <t>Permanently learn Ice Resistance</t>
-  </si>
-  <si>
-    <t>Magic Arrow</t>
-  </si>
-  <si>
-    <t>Permanently learn Magic Arrow</t>
-  </si>
-  <si>
-    <t>Permanently learn Strength</t>
-  </si>
-  <si>
-    <t>NameLevel</t>
-  </si>
-  <si>
-    <t>Leather Boots</t>
-  </si>
-  <si>
     <t>Boots</t>
   </si>
   <si>
@@ -333,12 +336,12 @@
     <t>Chainmail Bracers</t>
   </si>
   <si>
+    <t>Iron Bracers</t>
+  </si>
+  <si>
     <t>Leather Bracers</t>
   </si>
   <si>
-    <t>Metal Bracers</t>
-  </si>
-  <si>
     <t>Chain Mail Armor</t>
   </si>
   <si>
@@ -435,24 +438,24 @@
     <t>PermanentlyIncreaseStrength +1</t>
   </si>
   <si>
+    <t>Iron Gauntlets</t>
+  </si>
+  <si>
+    <t>Gauntlets</t>
+  </si>
+  <si>
     <t>Leather Gauntlets</t>
   </si>
   <si>
-    <t>Gauntlets</t>
-  </si>
-  <si>
-    <t>Metal Gauntlets</t>
+    <t>Iron Helment</t>
+  </si>
+  <si>
+    <t>Helment</t>
   </si>
   <si>
     <t>Leather Helment</t>
   </si>
   <si>
-    <t>Helment</t>
-  </si>
-  <si>
-    <t>Iron Helment</t>
-  </si>
-  <si>
     <t>Steel Helment</t>
   </si>
   <si>
@@ -597,7 +600,7 @@
     <t>Summon Monster III</t>
   </si>
   <si>
-    <t>Small Metal Sheild</t>
+    <t>Small Iron Sheild</t>
   </si>
   <si>
     <t>Shield</t>
@@ -1227,7 +1230,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1236,7 +1241,7 @@
     <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
@@ -1273,7 +1278,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -1291,18 +1296,18 @@
         <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B3">
         <v>30</v>
@@ -1320,18 +1325,18 @@
         <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -1349,18 +1354,18 @@
         <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B5">
         <v>18</v>
@@ -1378,18 +1383,18 @@
         <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B6">
         <v>28</v>
@@ -1407,18 +1412,18 @@
         <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -1436,18 +1441,18 @@
         <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1462,10 +1467,10 @@
         <v>3000</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
@@ -1473,7 +1478,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -1488,10 +1493,10 @@
         <v>3000</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I9" t="s">
         <v>30</v>
@@ -1499,7 +1504,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1514,10 +1519,10 @@
         <v>3000</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I10" t="s">
         <v>15</v>
@@ -1525,7 +1530,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1540,10 +1545,10 @@
         <v>3000</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I11" t="s">
         <v>36</v>
@@ -1551,7 +1556,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1566,18 +1571,18 @@
         <v>1600</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1592,18 +1597,18 @@
         <v>1600</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1618,18 +1623,18 @@
         <v>1600</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1638,24 +1643,24 @@
         <v>1</v>
       </c>
       <c r="D15">
+        <v>5000</v>
+      </c>
+      <c r="E15">
         <v>1000</v>
       </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I15" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1670,10 +1675,10 @@
         <v>1500</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I16" t="s">
         <v>23</v>
@@ -1681,7 +1686,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1696,18 +1701,18 @@
         <v>500</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -1722,10 +1727,10 @@
         <v>2400</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I18" t="s">
         <v>38</v>
@@ -1733,7 +1738,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1748,10 +1753,10 @@
         <v>2000</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
@@ -1759,7 +1764,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1774,10 +1779,10 @@
         <v>3000</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I20" t="s">
         <v>36</v>
@@ -1785,7 +1790,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1800,18 +1805,18 @@
         <v>6000</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1826,18 +1831,18 @@
         <v>2000</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -1852,18 +1857,18 @@
         <v>5000</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -1872,24 +1877,24 @@
         <v>40</v>
       </c>
       <c r="D24">
+        <v>3250</v>
+      </c>
+      <c r="E24">
         <v>2000</v>
       </c>
-      <c r="E24">
-        <v>85</v>
-      </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -1904,18 +1909,18 @@
         <v>1500</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I25" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -1933,15 +1938,15 @@
         <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I26" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1956,10 +1961,10 @@
         <v>1500</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G27" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I27" t="s">
         <v>15</v>
@@ -1967,7 +1972,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -1982,18 +1987,18 @@
         <v>500</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I28" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -2008,18 +2013,18 @@
         <v>500</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I29" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2034,10 +2039,10 @@
         <v>2500</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G30" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
@@ -2045,7 +2050,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2060,18 +2065,18 @@
         <v>500</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G31" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I31" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -2086,10 +2091,10 @@
         <v>1500</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G32" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I32" t="s">
         <v>15</v>
@@ -2097,7 +2102,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2112,10 +2117,10 @@
         <v>3000</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
@@ -2123,7 +2128,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -2138,18 +2143,18 @@
         <v>1000</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I34" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -2164,18 +2169,18 @@
         <v>1000</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -2190,18 +2195,18 @@
         <v>1000</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G36" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -2216,18 +2221,18 @@
         <v>1000</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G37" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2242,10 +2247,10 @@
         <v>1600</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I38" t="s">
         <v>11</v>
@@ -2253,7 +2258,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2268,10 +2273,10 @@
         <v>2000</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I39" t="s">
         <v>23</v>
@@ -2279,7 +2284,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2294,18 +2299,18 @@
         <v>750</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I40" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -2320,18 +2325,18 @@
         <v>15</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -2346,18 +2351,18 @@
         <v>15</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G42" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I42" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2372,13 +2377,13 @@
         <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G43" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I43" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2391,7 +2396,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2438,7 +2443,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -2453,21 +2458,21 @@
         <v>0.01</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2482,18 +2487,18 @@
         <v>0.01</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2508,10 +2513,10 @@
         <v>0.01</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -2519,7 +2524,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2534,10 +2539,10 @@
         <v>0.01</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -2553,7 +2558,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2591,24 +2596,24 @@
         <v>45</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -2623,16 +2628,16 @@
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2658,16 +2663,16 @@
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J3">
         <v>20</v>
@@ -2693,16 +2698,16 @@
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J4">
         <v>60</v>
@@ -2728,16 +2733,16 @@
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2763,16 +2768,16 @@
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J6">
         <v>60</v>
@@ -2798,16 +2803,16 @@
         <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J7">
         <v>60</v>
@@ -2833,16 +2838,16 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8" t="s">
         <v>174</v>
-      </c>
-      <c r="I8" t="s">
-        <v>173</v>
       </c>
       <c r="J8">
         <v>60</v>
@@ -2868,16 +2873,16 @@
         <v>150</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J9">
         <v>60</v>
@@ -2903,16 +2908,16 @@
         <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J10">
         <v>60</v>
@@ -2938,16 +2943,16 @@
         <v>150</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2973,16 +2978,16 @@
         <v>150</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -3008,16 +3013,16 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3028,7 +3033,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -3043,16 +3048,16 @@
         <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G14">
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3078,16 +3083,16 @@
         <v>150</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I15" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J15">
         <v>30</v>
@@ -3113,16 +3118,16 @@
         <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J16">
         <v>60</v>
@@ -3133,7 +3138,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -3148,16 +3153,16 @@
         <v>150</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J17">
         <v>60</v>
@@ -3183,13 +3188,13 @@
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
@@ -3203,7 +3208,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3218,16 +3223,16 @@
         <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -3253,16 +3258,16 @@
         <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J20">
         <v>60</v>
@@ -3273,7 +3278,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -3288,16 +3293,16 @@
         <v>150</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -3308,7 +3313,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B22">
         <v>5</v>
@@ -3323,16 +3328,16 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -3343,7 +3348,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B23">
         <v>7</v>
@@ -3358,16 +3363,16 @@
         <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -3386,7 +3391,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3421,15 +3426,15 @@
         <v>45</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -3444,7 +3449,7 @@
         <v>300</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -3470,7 +3475,7 @@
         <v>300</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -3496,7 +3501,7 @@
         <v>300</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -3522,7 +3527,7 @@
         <v>300</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -3548,7 +3553,7 @@
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -3574,7 +3579,7 @@
         <v>300</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -3600,7 +3605,7 @@
         <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -3626,7 +3631,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -3652,7 +3657,7 @@
         <v>300</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -3678,7 +3683,7 @@
         <v>300</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -3704,7 +3709,7 @@
         <v>300</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -3730,7 +3735,7 @@
         <v>300</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -3756,7 +3761,7 @@
         <v>300</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -3782,7 +3787,7 @@
         <v>300</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -3808,7 +3813,7 @@
         <v>300</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3834,7 +3839,7 @@
         <v>300</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -3853,7 +3858,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3888,15 +3893,15 @@
         <v>45</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -3911,10 +3916,10 @@
         <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3922,7 +3927,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -3937,10 +3942,10 @@
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3948,7 +3953,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -3963,10 +3968,10 @@
         <v>200</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3974,7 +3979,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -3989,10 +3994,10 @@
         <v>200</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -4000,7 +4005,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4015,10 +4020,10 @@
         <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -4026,7 +4031,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -4041,10 +4046,10 @@
         <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -4052,7 +4057,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4067,10 +4072,10 @@
         <v>200</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -4078,7 +4083,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4093,10 +4098,10 @@
         <v>200</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H9">
         <v>10</v>
@@ -4104,7 +4109,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4119,10 +4124,10 @@
         <v>200</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H10">
         <v>60</v>
@@ -4130,7 +4135,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4145,10 +4150,10 @@
         <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H11">
         <v>60</v>
@@ -4156,7 +4161,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4171,10 +4176,10 @@
         <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H12">
         <v>60</v>
@@ -4182,7 +4187,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -4197,10 +4202,10 @@
         <v>200</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H13">
         <v>60</v>
@@ -4208,7 +4213,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4223,10 +4228,10 @@
         <v>200</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -4234,7 +4239,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4249,10 +4254,10 @@
         <v>200</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H15">
         <v>60</v>
@@ -4260,7 +4265,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4275,10 +4280,10 @@
         <v>200</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H16">
         <v>60</v>
@@ -4294,7 +4299,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4331,16 +4336,16 @@
         <v>45</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4360,13 +4365,13 @@
         <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I2">
         <v>20</v>
@@ -4377,7 +4382,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4392,10 +4397,10 @@
         <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -4409,7 +4414,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4424,13 +4429,13 @@
         <v>200</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -4441,7 +4446,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4456,13 +4461,13 @@
         <v>200</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -4473,7 +4478,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -4488,13 +4493,13 @@
         <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -4513,7 +4518,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4573,21 +4578,21 @@
         <v>1500</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4602,21 +4607,21 @@
         <v>2500</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4631,21 +4636,21 @@
         <v>250</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -4660,79 +4665,79 @@
         <v>450</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="D6">
         <v>2000</v>
       </c>
       <c r="E6">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>2000</v>
       </c>
       <c r="E7">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4747,21 +4752,21 @@
         <v>10000</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I8">
         <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4776,21 +4781,21 @@
         <v>12000</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I9">
         <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4805,21 +4810,21 @@
         <v>5000</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I10">
         <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4834,21 +4839,21 @@
         <v>500</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -4863,21 +4868,21 @@
         <v>500</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -4892,21 +4897,21 @@
         <v>500</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I13">
         <v>6</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4921,137 +4926,137 @@
         <v>500</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
       <c r="E15">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>2000</v>
       </c>
       <c r="E16">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E17">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>500</v>
+      </c>
+      <c r="E18">
+        <v>500</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" t="s">
         <v>140</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>30</v>
-      </c>
-      <c r="D18">
-        <v>2000</v>
-      </c>
-      <c r="E18">
-        <v>2000</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" t="s">
-        <v>139</v>
-      </c>
       <c r="I18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5066,21 +5071,21 @@
         <v>2500</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I19">
         <v>9</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5095,21 +5100,21 @@
         <v>200</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -5124,21 +5129,21 @@
         <v>200</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I21">
         <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -5153,21 +5158,21 @@
         <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5182,21 +5187,21 @@
         <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I23">
         <v>2</v>
       </c>
       <c r="J23" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -5211,21 +5216,21 @@
         <v>500</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -5240,21 +5245,21 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I25">
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5269,16 +5274,16 @@
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G26" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -5291,7 +5296,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5532,7 +5537,7 @@
         <v>300</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
         <v>52</v>
@@ -5547,12 +5552,12 @@
         <v>35000</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -5567,7 +5572,7 @@
         <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
         <v>52</v>
@@ -5582,12 +5587,12 @@
         <v>35000</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -5605,7 +5610,7 @@
         <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -5622,7 +5627,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -5640,7 +5645,7 @@
         <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -5657,7 +5662,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -5672,10 +5677,10 @@
         <v>1000</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -5687,12 +5692,12 @@
         <v>8000</v>
       </c>
       <c r="K11" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5707,10 +5712,10 @@
         <v>800</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -5722,12 +5727,12 @@
         <v>5000</v>
       </c>
       <c r="K12" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -5742,10 +5747,10 @@
         <v>2500</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -5757,12 +5762,12 @@
         <v>20000</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -5777,10 +5782,10 @@
         <v>5000</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -5792,12 +5797,12 @@
         <v>50000</v>
       </c>
       <c r="K14" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -5812,10 +5817,10 @@
         <v>1500</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -5827,12 +5832,12 @@
         <v>15000</v>
       </c>
       <c r="K15" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -5847,10 +5852,10 @@
         <v>4000</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -5862,12 +5867,12 @@
         <v>35000</v>
       </c>
       <c r="K16" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5882,10 +5887,10 @@
         <v>500</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -5897,12 +5902,12 @@
         <v>10000</v>
       </c>
       <c r="K17" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -5917,10 +5922,10 @@
         <v>2850</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -5932,12 +5937,12 @@
         <v>22000</v>
       </c>
       <c r="K18" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5952,10 +5957,10 @@
         <v>300</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -5967,12 +5972,12 @@
         <v>5000</v>
       </c>
       <c r="K19" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -5987,10 +5992,10 @@
         <v>1000</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -6002,7 +6007,7 @@
         <v>12000</v>
       </c>
       <c r="K20" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -6014,8 +6019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>